<commit_message>
changes has been done logout and listners
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDATA/KnnectTestData1.xlsx
+++ b/src/test/resources/TestDATA/KnnectTestData1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91993\Desktop\BS\Kennect_Assignment\src\test\resources\TestDATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C5CAE8-44A3-491E-99A9-3A98845AC0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDF01C8-6379-488F-93A1-4E9BD34A379C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D3682EC6-9CFD-4F9A-9CDC-DF9F1FEBE971}"/>
+    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{D3682EC6-9CFD-4F9A-9CDC-DF9F1FEBE971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Mr. Ratan Singh</t>
-  </si>
-  <si>
     <t>test@kennect.io</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>Mr. Indra Singh</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74497BB9-7B32-485C-A892-39CA445B7A35}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
@@ -585,13 +587,13 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="D2" s="2">
         <v>168</v>
@@ -615,7 +617,7 @@
         <v>16</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>17</v>
@@ -624,13 +626,13 @@
         <v>18</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>